<commit_message>
Deploy samply/bbmri-fhir-ig to github.com/samply/bbmri-fhir-ig.git:gh-pages
</commit_message>
<xml_diff>
--- a/StructureDefinition-Biobank.xlsx
+++ b/StructureDefinition-Biobank.xlsx
@@ -1291,8 +1291,8 @@
   </si>
   <si>
     <t>&lt;valuePeriod xmlns="http://hl7.org/fhir"&gt;
-  &lt;start value="2010-03-23T00:00:00+00:00"/&gt;
-  &lt;end value="2010-07-01T00:00:00+00:00"/&gt;
+  &lt;start value="2010-03-23"/&gt;
+  &lt;end value="2010-07-01"/&gt;
 &lt;/valuePeriod&gt;</t>
   </si>
   <si>

</xml_diff>